<commit_message>
update note of 'attribute'
</commit_message>
<xml_diff>
--- a/26_AssemblyLanguage/5_StorageOfStruct/Storage of Struct.xlsx
+++ b/26_AssemblyLanguage/5_StorageOfStruct/Storage of Struct.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage\5_StorageOfStruct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA0EDDA-D18E-4699-9175-92B9D5DF7730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4586ADE7-FE0F-4465-9C8A-6A166CDF93B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>0x10</t>
   </si>
@@ -108,6 +108,32 @@
     <t>1，char占一个byte，short占两个byte。所以a后面有个填充位，为了和 short b对齐；
 2，为什么后面也要加3个填充位？
 原因movl这样的指令应当访问的地址是4的位数，是为了保证整个结构体的内存容量是4的倍数，保证访问效率。后面的数据就可以紧挨着他后面排列，这样就不用担心不是4的倍数了。</t>
+  </si>
+  <si>
+    <t>siseof 结果8</t>
+  </si>
+  <si>
+    <t>StorageOfStruct02.c
+调整声明变量的顺序后节省了4 bytes的空间，而且是节省的寄存器的空间，可见理解底层内存布局是多么重要。</t>
+  </si>
+  <si>
+    <t>char a</t>
+  </si>
+  <si>
+    <t>short b</t>
+  </si>
+  <si>
+    <t>int c</t>
+  </si>
+  <si>
+    <t>char d</t>
+  </si>
+  <si>
+    <t>No padding</t>
+  </si>
+  <si>
+    <t>The size of a stuct variable is not the mutiple of 4 after using "attribute". 
+So the visiting speed is going to be slower.</t>
   </si>
 </sst>
 </file>
@@ -173,23 +199,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -614,146 +646,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="E5:U27"/>
+  <dimension ref="E5:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S25" sqref="S25"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31:N41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="17" max="17" width="23.5703125" customWidth="1"/>
     <col min="21" max="21" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="5:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+      <c r="Z6" s="4"/>
+    </row>
+    <row r="7" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
+    </row>
+    <row r="8" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="4"/>
+    </row>
+    <row r="9" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V9" s="4"/>
+      <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
+      <c r="Z9" s="4"/>
+    </row>
+    <row r="10" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H10" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V10" s="4"/>
+      <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
+      <c r="Z10" s="4"/>
+    </row>
+    <row r="11" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V11" s="4"/>
+      <c r="W11" s="4"/>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4"/>
+      <c r="Z11" s="4"/>
+    </row>
+    <row r="12" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="5:20" x14ac:dyDescent="0.25">
+      <c r="V12" s="4"/>
+      <c r="W12" s="4"/>
+      <c r="X12" s="4"/>
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4"/>
+    </row>
+    <row r="13" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
@@ -763,89 +833,113 @@
       <c r="J13" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E14" s="4" t="s">
+      <c r="V13" s="4"/>
+      <c r="W13" s="4"/>
+      <c r="X13" s="4"/>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4"/>
+    </row>
+    <row r="14" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="4"/>
+      <c r="F14" s="3"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+    </row>
+    <row r="15" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="5:20" x14ac:dyDescent="0.25">
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="4"/>
+      <c r="X15" s="4"/>
+      <c r="Y15" s="4"/>
+      <c r="Z15" s="4"/>
+    </row>
+    <row r="16" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
+      <c r="J16" s="5"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+    </row>
+    <row r="17" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="H17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="J17" s="5"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="5"/>
       <c r="S17" s="1" t="s">
         <v>20</v>
       </c>
@@ -855,40 +949,51 @@
       <c r="U17" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="4"/>
+      <c r="X17" s="4"/>
+      <c r="Y17" s="4"/>
+      <c r="Z17" s="4"/>
+    </row>
+    <row r="18" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="5"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+    </row>
+    <row r="19" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
+      <c r="J19" s="5"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
       <c r="S19" s="1" t="s">
         <v>18</v>
       </c>
@@ -898,19 +1003,24 @@
       <c r="U19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="V19" s="4"/>
+      <c r="W19" s="4"/>
+      <c r="X19" s="4"/>
+      <c r="Y19" s="4"/>
+      <c r="Z19" s="4"/>
+    </row>
+    <row r="20" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
       <c r="S20" s="1" t="s">
         <v>21</v>
       </c>
@@ -921,7 +1031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H21" s="1" t="s">
         <v>17</v>
       </c>
@@ -931,11 +1041,11 @@
       <c r="J21" t="s">
         <v>16</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
       <c r="S21" s="1" t="s">
         <v>17</v>
       </c>
@@ -943,54 +1053,231 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:26" x14ac:dyDescent="0.25">
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:26" x14ac:dyDescent="0.25">
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:26" x14ac:dyDescent="0.25">
       <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
     </row>
-    <row r="25" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="5:26" x14ac:dyDescent="0.25">
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
       <c r="P25" s="2"/>
     </row>
-    <row r="26" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:26" x14ac:dyDescent="0.25">
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="5:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="H27" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
+    <row r="29" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="H31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="5:26" x14ac:dyDescent="0.25">
+      <c r="H32" s="1"/>
+      <c r="I32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H33" s="1"/>
+      <c r="I33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H34" s="1"/>
+      <c r="I34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H35" s="1"/>
+      <c r="I35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H36" s="1"/>
+      <c r="I36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H37" s="1"/>
+      <c r="I37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H38" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J42" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H44" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
+    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="K31:N41"/>
+    <mergeCell ref="V6:Z19"/>
     <mergeCell ref="J14:J17"/>
     <mergeCell ref="J18:J19"/>
     <mergeCell ref="E14:F18"/>
     <mergeCell ref="L5:P21"/>
+    <mergeCell ref="Q16:Q18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update note of C
</commit_message>
<xml_diff>
--- a/26_AssemblyLanguage/5_StorageOfStruct/Storage of Struct.xlsx
+++ b/26_AssemblyLanguage/5_StorageOfStruct/Storage of Struct.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Private Files\Computer\C-Code\26_AssemblyLanguage\5_StorageOfStruct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4586ADE7-FE0F-4465-9C8A-6A166CDF93B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9718683D-B2BF-402E-A352-C9283C46FC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>0x10</t>
   </si>
@@ -103,37 +103,40 @@
   </si>
   <si>
     <t>sizeof结果为12，说明d后面有三个填充位</t>
+  </si>
+  <si>
+    <t>siseof 结果8</t>
+  </si>
+  <si>
+    <t>StorageOfStruct02.c
+调整声明变量的顺序后节省了4 bytes的空间，而且是节省的寄存器的空间，可见理解底层内存布局是多么重要。</t>
+  </si>
+  <si>
+    <t>char a</t>
+  </si>
+  <si>
+    <t>short b</t>
+  </si>
+  <si>
+    <t>int c</t>
+  </si>
+  <si>
+    <t>char d</t>
+  </si>
+  <si>
+    <t>No padding</t>
+  </si>
+  <si>
+    <t>The size of a stuct variable is not the mutiple of 4 after using "attribute". 
+So the visiting speed is going to be slower.</t>
   </si>
   <si>
     <t>1，char占一个byte，short占两个byte。所以a后面有个填充位，为了和 short b对齐；
 2，为什么后面也要加3个填充位？
-原因movl这样的指令应当访问的地址是4的位数，是为了保证整个结构体的内存容量是4的倍数，保证访问效率。后面的数据就可以紧挨着他后面排列，这样就不用担心不是4的倍数了。</t>
-  </si>
-  <si>
-    <t>siseof 结果8</t>
-  </si>
-  <si>
-    <t>StorageOfStruct02.c
-调整声明变量的顺序后节省了4 bytes的空间，而且是节省的寄存器的空间，可见理解底层内存布局是多么重要。</t>
-  </si>
-  <si>
-    <t>char a</t>
-  </si>
-  <si>
-    <t>short b</t>
-  </si>
-  <si>
-    <t>int c</t>
-  </si>
-  <si>
-    <t>char d</t>
-  </si>
-  <si>
-    <t>No padding</t>
-  </si>
-  <si>
-    <t>The size of a stuct variable is not the mutiple of 4 after using "attribute". 
-So the visiting speed is going to be slower.</t>
+原因movl这样的指令应当访问的地址是4的位数，是为了保证整个结构体的内存容量是4的倍数，保证访问效率。后面的数据就可以紧挨着他后面排列，这样就不用担心不是4的倍数了。使用4*index (0,1,...)这样的下标时访问速度会很高。</t>
+  </si>
+  <si>
+    <t>index</t>
   </si>
 </sst>
 </file>
@@ -206,6 +209,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -219,9 +225,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="E5:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31:N41"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,13 +666,13 @@
       <c r="I5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
+      <c r="L5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1" t="s">
         <v>15</v>
@@ -680,82 +683,82 @@
       <c r="I6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
-      <c r="Z6" s="4"/>
+      <c r="V6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
     </row>
     <row r="7" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
-      <c r="Y7" s="4"/>
-      <c r="Z7" s="4"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
     </row>
     <row r="8" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
-      <c r="Y9" s="4"/>
-      <c r="Z9" s="4"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="5"/>
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="5"/>
     </row>
     <row r="10" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H10" s="1" t="s">
@@ -764,20 +767,20 @@
       <c r="I10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
-      <c r="Y10" s="4"/>
-      <c r="Z10" s="4"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+      <c r="X10" s="5"/>
+      <c r="Y10" s="5"/>
+      <c r="Z10" s="5"/>
     </row>
     <row r="11" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="s">
@@ -786,20 +789,20 @@
       <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="5"/>
     </row>
     <row r="12" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H12" s="1" t="s">
@@ -808,20 +811,20 @@
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+      <c r="Z12" s="5"/>
     </row>
     <row r="13" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H13" s="1" t="s">
@@ -833,113 +836,113 @@
       <c r="J13" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
+      <c r="V13" s="5"/>
+      <c r="W13" s="5"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="5"/>
+      <c r="Z13" s="5"/>
     </row>
     <row r="14" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="4"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
+      <c r="V14" s="5"/>
+      <c r="W14" s="5"/>
+      <c r="X14" s="5"/>
+      <c r="Y14" s="5"/>
+      <c r="Z14" s="5"/>
     </row>
     <row r="15" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="5"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
+      <c r="J15" s="6"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
-      <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
+      <c r="V15" s="5"/>
+      <c r="W15" s="5"/>
+      <c r="X15" s="5"/>
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="5"/>
     </row>
     <row r="16" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J16" s="5"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="5" t="s">
-        <v>27</v>
+      <c r="J16" s="6"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="S16" s="1"/>
       <c r="T16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
-      <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
+      <c r="V16" s="5"/>
+      <c r="W16" s="5"/>
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5"/>
+      <c r="Z16" s="5"/>
     </row>
     <row r="17" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="H17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="5"/>
+      <c r="J17" s="6"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="6"/>
       <c r="S17" s="1" t="s">
         <v>20</v>
       </c>
@@ -949,37 +952,37 @@
       <c r="U17" t="s">
         <v>22</v>
       </c>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
-      <c r="Y17" s="4"/>
-      <c r="Z17" s="4"/>
+      <c r="V17" s="5"/>
+      <c r="W17" s="5"/>
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5"/>
+      <c r="Z17" s="5"/>
     </row>
     <row r="18" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="5"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="6"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="V18" s="5"/>
+      <c r="W18" s="5"/>
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5"/>
+      <c r="Z18" s="5"/>
     </row>
     <row r="19" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H19" s="1" t="s">
@@ -988,12 +991,12 @@
       <c r="I19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J19" s="5"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="7"/>
+      <c r="J19" s="6"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
       <c r="S19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1003,11 +1006,11 @@
       <c r="U19" t="s">
         <v>19</v>
       </c>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H20" s="1" t="s">
@@ -1016,11 +1019,11 @@
       <c r="I20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="7"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
       <c r="S20" s="1" t="s">
         <v>21</v>
       </c>
@@ -1041,11 +1044,11 @@
       <c r="J21" t="s">
         <v>16</v>
       </c>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="7"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
       <c r="S21" s="1" t="s">
         <v>17</v>
       </c>
@@ -1089,11 +1092,11 @@
       <c r="P26" s="2"/>
     </row>
     <row r="27" spans="5:26" x14ac:dyDescent="0.25">
-      <c r="H27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
+      <c r="H27" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -1117,74 +1120,89 @@
       <c r="I31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
+      <c r="K31" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
     </row>
     <row r="32" spans="5:26" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
       <c r="I32" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
       <c r="H33" s="1"/>
       <c r="I33" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>-11</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>-10</v>
+      </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="3"/>
-    </row>
-    <row r="36" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>-9</v>
+      </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-    </row>
-    <row r="37" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>-8</v>
+      </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="3"/>
-    </row>
-    <row r="38" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>-7</v>
+      </c>
       <c r="H38" s="1" t="s">
         <v>21</v>
       </c>
@@ -1192,44 +1210,56 @@
         <v>7</v>
       </c>
       <c r="J38" t="s">
-        <v>32</v>
-      </c>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-    </row>
-    <row r="39" spans="8:14" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>-6</v>
+      </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-    </row>
-    <row r="40" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>-5</v>
+      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="3"/>
-    </row>
-    <row r="41" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+    </row>
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>-4</v>
+      </c>
       <c r="H41" s="1"/>
       <c r="I41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-    </row>
-    <row r="42" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+    </row>
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>-3</v>
+      </c>
       <c r="H42" s="1" t="s">
         <v>20</v>
       </c>
@@ -1237,16 +1267,22 @@
         <v>3</v>
       </c>
       <c r="J42" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="43" spans="8:14" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <v>-2</v>
+      </c>
       <c r="H43" s="1"/>
       <c r="I43" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <v>-1</v>
+      </c>
       <c r="H44" s="1" t="s">
         <v>18</v>
       </c>
@@ -1254,10 +1290,16 @@
         <v>1</v>
       </c>
       <c r="J44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="8:14" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
+        <v>35</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
       <c r="H45" s="1" t="s">
         <v>17</v>
       </c>
@@ -1265,19 +1307,19 @@
         <v>0</v>
       </c>
       <c r="J45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E14:F18"/>
+    <mergeCell ref="L5:P21"/>
+    <mergeCell ref="Q16:Q18"/>
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="K31:N41"/>
     <mergeCell ref="V6:Z19"/>
     <mergeCell ref="J14:J17"/>
     <mergeCell ref="J18:J19"/>
-    <mergeCell ref="E14:F18"/>
-    <mergeCell ref="L5:P21"/>
-    <mergeCell ref="Q16:Q18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>